<commit_message>
Conor helped me bugtest :)
</commit_message>
<xml_diff>
--- a/ABC_PG.xlsx
+++ b/ABC_PG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiademedeiros/PycharmProjects/Imports/ABC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE23AD18-734A-B746-90F8-A1409DC7395F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20802961-E68C-A746-BAD3-EEF7A0A4C7B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14000" activeTab="7" xr2:uid="{249E6F38-37D1-C84F-B756-4419E072FBD0}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="191">
   <si>
     <t>item</t>
   </si>
@@ -460,9 +460,6 @@
     <t>You are standing in front of Adelaide's Battle Café, known colloquially as ABC, a café renowned throughout the Necropolis as a place for witches to pitch their familiars against each other in a spirit battle over a cup of coffee. On the street in front of the café are a &gt;stray skelekitty&lt;, and a &gt;vampire kid&lt; standing on tip-toe as they try to look through the shop window into the hustle and bustle within.</t>
   </si>
   <si>
-    <t>&gt;Frank and Stein&lt; are both standing behind the bar,and there are no other customers currently here.</t>
-  </si>
-  <si>
     <t>A stray skelekitty you picked up off the street</t>
   </si>
   <si>
@@ -586,9 +583,6 @@
     <t>"Don't waste my time, human" the frog says, looking up from his potion. "The key is yours."</t>
   </si>
   <si>
-    <t>The frog wizard takes the tooth right out of your hand with a flick of his tongue, and drops it into the bathtub, which begins to effervesce violently. "Yes, excellent…" he mumbles, no longer interested in you.</t>
-  </si>
-  <si>
     <t>"Pah!" the frog says, as you hold the spirit nip out to him. "You think that would work on *me*?"</t>
   </si>
   <si>
@@ -608,6 +602,18 @@
   </si>
   <si>
     <t>flyer, flyers</t>
+  </si>
+  <si>
+    <t>&gt;Frank and Stein&lt; are both standing behind the bar, and there are no other customers currently here.</t>
+  </si>
+  <si>
+    <t>You find yourself suddenly out of character (OC)!</t>
+  </si>
+  <si>
+    <t>frog_occupied</t>
+  </si>
+  <si>
+    <t>The frog wizard takes the tooth right out of your hand with a flick of his tongue, and drops it into the bathtub, which begins to effervesce violently. "Yes, excellent…" he mumbles, and produces a key in mid-air which he hands to you in return.</t>
   </si>
 </sst>
 </file>
@@ -967,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78240EAD-4701-0E4D-9714-E61B1AD393AF}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView zoomScale="187" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1053,7 +1059,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B9">
         <v>12</v>
@@ -1067,12 +1073,17 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -1085,7 +1096,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1175,10 +1186,10 @@
         <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F4" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="G4" t="s">
         <v>95</v>
@@ -1192,19 +1203,19 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
       </c>
       <c r="E5" t="s">
+        <v>172</v>
+      </c>
+      <c r="F5" t="s">
         <v>173</v>
       </c>
-      <c r="F5" t="s">
-        <v>174</v>
-      </c>
       <c r="G5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H5" t="s">
         <v>13</v>
@@ -1224,13 +1235,13 @@
         <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G6" t="s">
         <v>94</v>
       </c>
       <c r="H6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1238,16 +1249,16 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C7" t="s">
         <v>71</v>
       </c>
       <c r="E7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7" t="s">
         <v>159</v>
-      </c>
-      <c r="F7" t="s">
-        <v>160</v>
       </c>
       <c r="G7" t="s">
         <v>96</v>
@@ -1258,13 +1269,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" t="s">
         <v>152</v>
-      </c>
-      <c r="F8" t="s">
-        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1347,13 +1361,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7" t="s">
         <v>170</v>
-      </c>
-      <c r="B7" t="s">
-        <v>172</v>
-      </c>
-      <c r="C7" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1361,7 +1375,7 @@
         <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C8" t="s">
         <v>90</v>
@@ -1372,7 +1386,7 @@
         <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C9" t="s">
         <v>91</v>
@@ -1391,10 +1405,10 @@
         <v>94</v>
       </c>
       <c r="B11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1407,7 +1421,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView zoomScale="183" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1446,13 +1460,13 @@
         <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1466,7 +1480,7 @@
         <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F3">
         <v>7</v>
@@ -1545,16 +1559,16 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E8" t="s">
         <v>144</v>
-      </c>
-      <c r="E8" t="s">
-        <v>145</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1589,7 +1603,7 @@
         <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E1" t="s">
         <v>89</v>
@@ -1628,7 +1642,7 @@
         <v>102</v>
       </c>
       <c r="C4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1647,7 +1661,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C6" t="s">
         <v>101</v>
@@ -1655,16 +1669,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" t="s">
         <v>175</v>
       </c>
-      <c r="C7" t="s">
-        <v>176</v>
-      </c>
       <c r="D7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1672,10 +1686,10 @@
         <v>94</v>
       </c>
       <c r="B8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
@@ -1690,7 +1704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA03647-6A0D-DD44-B6FA-3A3FFECA1E89}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScale="141" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="141" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1711,7 +1725,7 @@
         <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -1725,7 +1739,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1767,13 +1781,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" t="s">
         <v>177</v>
-      </c>
-      <c r="C5" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1799,7 +1813,7 @@
         <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1818,7 +1832,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -1875,10 +1889,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1892,7 +1906,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="194" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1916,10 +1930,10 @@
         <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1947,7 +1961,7 @@
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1997,10 +2011,13 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C7" t="s">
-        <v>181</v>
+        <v>190</v>
+      </c>
+      <c r="E7" t="s">
+        <v>189</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -2081,10 +2098,10 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -2159,10 +2176,10 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -2240,10 +2257,10 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D25" t="b">
         <v>1</v>
@@ -2299,7 +2316,7 @@
         <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -2321,10 +2338,10 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C31" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D31" t="b">
         <v>1</v>
@@ -2405,10 +2422,10 @@
         <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C37" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D37" t="b">
         <v>1</v>
@@ -2422,10 +2439,10 @@
         <v>2</v>
       </c>
       <c r="C38" t="s">
+        <v>141</v>
+      </c>
+      <c r="E38" t="s">
         <v>142</v>
-      </c>
-      <c r="E38" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>